<commit_message>
code cleanup and completion of "level 1" historical ownership chains
</commit_message>
<xml_diff>
--- a/BvIDexport.xlsx
+++ b/BvIDexport.xlsx
@@ -12,381 +12,510 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t xml:space="preserve">NewBvDIDs</t>
   </si>
   <si>
+    <t xml:space="preserve">FR542051180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5110206610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US142546192L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB12133117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5330000056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE6270139382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE4010000539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR180020026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5110426441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5050471540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2151574829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5030088293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5190434206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8330415355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE6070009834</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESB98338411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL811655650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB*908439227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE5564620887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5170178473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM45532R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO988470937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5050567293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5030319504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE3170295464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB41239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5030456699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LULB201907</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO863769132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR531330389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB01142830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB13116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2190001854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2290291348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US870698303</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESA08001851</t>
   </si>
   <si>
-    <t xml:space="preserve">DE3170295464</t>
+    <t xml:space="preserve">DK10103940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5110426307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE6070491599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US133413761L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2210163123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT9110778886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KY*110014084853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE5560362138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESA28119220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2370010537</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ29259428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB00102498</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LULB195709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESB82056748</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7170000175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZA196701303806</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE5567818314</t>
   </si>
   <si>
     <t xml:space="preserve">DE6150261280</t>
   </si>
   <si>
+    <t xml:space="preserve">CHCHE112112310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2050372206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2150918982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBGG46130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE3070183858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE3070407436</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5050056484</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2011364466</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESA28157360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT04732570967</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7170311222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2350060811</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CYC307511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB15469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN0008687067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE6150007515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL012149187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT06312510966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL53748662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8190350014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8170504074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5110304100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7230282328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KY31377PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US150238465L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8170725443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2151253621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHCHE109101085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US411724239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8070234353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US541163725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2150965540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE75019980</t>
+  </si>
+  <si>
     <t xml:space="preserve">AT9150100345</t>
   </si>
   <si>
+    <t xml:space="preserve">DE5110066894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB04043908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR443837331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2350113248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHCHE114669799</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8310297852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBLP011863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT10236451000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2011425555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LULB104637</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL33292246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBGG50009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2230133950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7110175411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KY*110179911376</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7330620677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT00811720580</t>
+  </si>
+  <si>
     <t xml:space="preserve">NL01178978</t>
   </si>
   <si>
-    <t xml:space="preserve">DE2011425555</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK10103940</t>
+    <t xml:space="preserve">RU00040778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ00260428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL34108286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE*929123061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2190331916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE6290207493</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS6306051210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2250063387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2050488817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB02989338</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE6070524807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US363145972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7370113108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO987059699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE4070408675</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB23470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2250132994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE4170123108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU17230282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR552081317</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB13584</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US149185809L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8290178515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR379677636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBOC303117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEI1007130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR*J00S1080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB03039100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5110216866</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7330530056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IE008610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8170600335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE*820975510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5110001494</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR542008677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH0000049173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7010228841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8190010796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2010198197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU10625790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ41692918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2010378297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2030006515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB13109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO912230252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB13306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI06353667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESG08171118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US341843785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR380415125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB03586615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE*J00S1100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB13172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB48901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB02020410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7330029432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB02366963</t>
   </si>
   <si>
     <t xml:space="preserve">DE6070002888</t>
   </si>
   <si>
-    <t xml:space="preserve">FR180020026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7110175411</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHCHE112112310</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5110426307</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8170600335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ41692918</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5110206610</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ00260428</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7170311222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LULB104637</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2010378297</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE4070408675</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE*820975510</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5110066894</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB23470</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5030456699</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LULB201907</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5050471540</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2030006515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB13172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8190350014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE6070491599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB48901</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB04043908</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB41239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO863769132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR531330389</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB13109</t>
+    <t xml:space="preserve">DEFEI1007380</t>
   </si>
   <si>
     <t xml:space="preserve">FI02459755</t>
   </si>
   <si>
-    <t xml:space="preserve">DE2151253621</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB01142830</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB13116</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBGG50009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US133413761L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBGG46130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2190331916</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHCHE109101085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2210163123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2230133950</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR379677636</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2250063387</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AT9110778886</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2290291348</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBOC303117</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE3070183858</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KY*110014084853</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2050488817</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR*J00S1080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE5560362138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN0008687067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESA28119220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE3070407436</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2151574829</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE6150007515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB03586615</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2250132994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB00102498</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB13584</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5050056484</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO912230252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8070234353</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE5564620887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL012149187</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7010228841</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHCHE114669799</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5170178473</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB03039100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5190434206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5110304100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5110216866</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESB82056748</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5330000056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB02020410</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE*J00S1100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE6070524807</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KY*110179911376</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8190010796</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB13306</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7330530056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE6270139382</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7330029432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7330620677</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE6290207493</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US363145972</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2010198197</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7170000175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IS6306051210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7230282328</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5110001494</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR542051180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US541163725</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FI06353667</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7370113108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE008610</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8290178515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US150238465L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEI1007380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZA196701303806</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8310297852</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8170725443</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBLP011863</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE75019980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESG08171118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESB98338411</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR542008677</t>
-  </si>
-  <si>
     <t xml:space="preserve">GB03690065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US341843785</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB02366963</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BM45532R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR380415125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HU10625790</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT04732570967</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT06312510966</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO988470937</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL811655650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR552081317</t>
   </si>
 </sst>
 </file>
@@ -1343,6 +1472,221 @@
         <v>124</v>
       </c>
     </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Very large commit. Added a lot of data and scripts to get insight about effecive tax rates, labor productivity and capital productivity of firms depending on their ownership profile. Also added deeper information about network positions of firms and countries, statistics about coocurences and preferred conduit nations. Corrected some minor mistakes and weird code. Next step is going to be a regression model. I am still looking for proper variables. However, I will do that after a lot of writing on the actual thesis.
</commit_message>
<xml_diff>
--- a/BvIDexport.xlsx
+++ b/BvIDexport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
   <si>
     <t xml:space="preserve">NewBvDIDs</t>
   </si>
@@ -23,103 +23,112 @@
     <t xml:space="preserve">DE5110206610</t>
   </si>
   <si>
+    <t xml:space="preserve">DE5330000056</t>
+  </si>
+  <si>
     <t xml:space="preserve">US142546192L</t>
   </si>
   <si>
     <t xml:space="preserve">GB12133117</t>
   </si>
   <si>
-    <t xml:space="preserve">DE5330000056</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE6270139382</t>
   </si>
   <si>
+    <t xml:space="preserve">DE5110426441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5190434206</t>
+  </si>
+  <si>
     <t xml:space="preserve">DE4010000539</t>
   </si>
   <si>
+    <t xml:space="preserve">DE5030088293</t>
+  </si>
+  <si>
     <t xml:space="preserve">FR180020026</t>
   </si>
   <si>
-    <t xml:space="preserve">DE5110426441</t>
+    <t xml:space="preserve">DE8330415355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL811655650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESB98338411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2151574829</t>
   </si>
   <si>
     <t xml:space="preserve">DE5050471540</t>
   </si>
   <si>
-    <t xml:space="preserve">DE2151574829</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5030088293</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5190434206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8330415355</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE6070009834</t>
   </si>
   <si>
-    <t xml:space="preserve">ESB98338411</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL811655650</t>
-  </si>
-  <si>
     <t xml:space="preserve">GB*908439227</t>
   </si>
   <si>
+    <t xml:space="preserve">DE5050567293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO988470937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5170178473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5030319504</t>
+  </si>
+  <si>
     <t xml:space="preserve">SE5564620887</t>
   </si>
   <si>
-    <t xml:space="preserve">DE5170178473</t>
-  </si>
-  <si>
     <t xml:space="preserve">BM45532R</t>
   </si>
   <si>
-    <t xml:space="preserve">NO988470937</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5050567293</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5030319504</t>
+    <t xml:space="preserve">NO863769132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2190001854</t>
   </si>
   <si>
     <t xml:space="preserve">DE3170295464</t>
   </si>
   <si>
+    <t xml:space="preserve">GB01142830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US870698303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LULB201907</t>
+  </si>
+  <si>
     <t xml:space="preserve">DEFEB41239</t>
   </si>
   <si>
     <t xml:space="preserve">DE5030456699</t>
   </si>
   <si>
-    <t xml:space="preserve">LULB201907</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO863769132</t>
+    <t xml:space="preserve">DEFEB13116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2290291348</t>
   </si>
   <si>
     <t xml:space="preserve">FR531330389</t>
   </si>
   <si>
-    <t xml:space="preserve">GB01142830</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB13116</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2190001854</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2290291348</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US870698303</t>
+    <t xml:space="preserve">DE5110426307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2370010537</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE5560362138</t>
   </si>
   <si>
     <t xml:space="preserve">ESA08001851</t>
@@ -128,85 +137,94 @@
     <t xml:space="preserve">DK10103940</t>
   </si>
   <si>
-    <t xml:space="preserve">DE5110426307</t>
+    <t xml:space="preserve">KY*110014084853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ29259428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZA196701303806</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESB82056748</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE5567818314</t>
   </si>
   <si>
     <t xml:space="preserve">DE6070491599</t>
   </si>
   <si>
+    <t xml:space="preserve">DE2210163123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT9110778886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESA28119220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB00102498</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LULB195709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7170000175</t>
+  </si>
+  <si>
     <t xml:space="preserve">US133413761L</t>
   </si>
   <si>
-    <t xml:space="preserve">DE2210163123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AT9110778886</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KY*110014084853</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE5560362138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESA28119220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2370010537</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ29259428</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB00102498</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LULB195709</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESB82056748</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7170000175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZA196701303806</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE5567818314</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE6150261280</t>
   </si>
   <si>
+    <t xml:space="preserve">DE2011364466</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT04732570967</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHCHE112112310</t>
   </si>
   <si>
     <t xml:space="preserve">DE2050372206</t>
   </si>
   <si>
+    <t xml:space="preserve">DE8170000724</t>
+  </si>
+  <si>
     <t xml:space="preserve">DE2150918982</t>
   </si>
   <si>
+    <t xml:space="preserve">DE3070183858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE3070407436</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5050056484</t>
+  </si>
+  <si>
     <t xml:space="preserve">GBGG46130</t>
   </si>
   <si>
-    <t xml:space="preserve">DE3070183858</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE3070407436</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE5050056484</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2011364466</t>
-  </si>
-  <si>
     <t xml:space="preserve">ESA28157360</t>
   </si>
   <si>
-    <t xml:space="preserve">IT04732570967</t>
+    <t xml:space="preserve">DE6150007515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB15469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL012149187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CYC307511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT06312510966</t>
   </si>
   <si>
     <t xml:space="preserve">DE7170311222</t>
@@ -215,46 +233,37 @@
     <t xml:space="preserve">DE2350060811</t>
   </si>
   <si>
-    <t xml:space="preserve">CYC307511</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB15469</t>
-  </si>
-  <si>
     <t xml:space="preserve">IN0008687067</t>
   </si>
   <si>
-    <t xml:space="preserve">DE6150007515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL012149187</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT06312510966</t>
+    <t xml:space="preserve">DE8190350014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7230282328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8170504074</t>
   </si>
   <si>
     <t xml:space="preserve">NL53748662</t>
   </si>
   <si>
-    <t xml:space="preserve">DE8190350014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8170504074</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE5110304100</t>
   </si>
   <si>
-    <t xml:space="preserve">DE7230282328</t>
+    <t xml:space="preserve">US150238465L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8170725443</t>
   </si>
   <si>
     <t xml:space="preserve">KY31377PC</t>
   </si>
   <si>
-    <t xml:space="preserve">US150238465L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8170725443</t>
+    <t xml:space="preserve">US411724239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE75019980</t>
   </si>
   <si>
     <t xml:space="preserve">DE2151253621</t>
@@ -263,55 +272,61 @@
     <t xml:space="preserve">CHCHE109101085</t>
   </si>
   <si>
-    <t xml:space="preserve">US411724239</t>
+    <t xml:space="preserve">US541163725</t>
   </si>
   <si>
     <t xml:space="preserve">DE8070234353</t>
   </si>
   <si>
-    <t xml:space="preserve">US541163725</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE2150965540</t>
   </si>
   <si>
-    <t xml:space="preserve">EE75019980</t>
+    <t xml:space="preserve">FR443837331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5110066894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE5070255751</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBLP011863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT10236451000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2250192021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB04043908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2350113248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE8310297852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHCHE114669799</t>
   </si>
   <si>
     <t xml:space="preserve">AT9150100345</t>
   </si>
   <si>
-    <t xml:space="preserve">DE5110066894</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB04043908</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR443837331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2350113248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHCHE114669799</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE8310297852</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBLP011863</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT10236451000</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE2011425555</t>
   </si>
   <si>
+    <t xml:space="preserve">NL33292246</t>
+  </si>
+  <si>
     <t xml:space="preserve">LULB104637</t>
   </si>
   <si>
-    <t xml:space="preserve">NL33292246</t>
+    <t xml:space="preserve">IT00811720580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7110175411</t>
   </si>
   <si>
     <t xml:space="preserve">GBGG50009</t>
@@ -320,78 +335,72 @@
     <t xml:space="preserve">DE2230133950</t>
   </si>
   <si>
-    <t xml:space="preserve">DE7110175411</t>
-  </si>
-  <si>
     <t xml:space="preserve">KY*110179911376</t>
   </si>
   <si>
     <t xml:space="preserve">DE7330620677</t>
   </si>
   <si>
-    <t xml:space="preserve">IT00811720580</t>
-  </si>
-  <si>
     <t xml:space="preserve">NL01178978</t>
   </si>
   <si>
+    <t xml:space="preserve">DE*929123061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL34108286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2190331916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ00260428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE6290207493</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS6306051210</t>
+  </si>
+  <si>
     <t xml:space="preserve">RU00040778</t>
   </si>
   <si>
-    <t xml:space="preserve">CZ00260428</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NL34108286</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE*929123061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2190331916</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE6290207493</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IS6306051210</t>
+    <t xml:space="preserve">NO987059699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB02989338</t>
   </si>
   <si>
     <t xml:space="preserve">DE2250063387</t>
   </si>
   <si>
+    <t xml:space="preserve">DE7370113108</t>
+  </si>
+  <si>
     <t xml:space="preserve">DE2050488817</t>
   </si>
   <si>
-    <t xml:space="preserve">GB02989338</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE6070524807</t>
   </si>
   <si>
     <t xml:space="preserve">US363145972</t>
   </si>
   <si>
-    <t xml:space="preserve">DE7370113108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO987059699</t>
+    <t xml:space="preserve">RU17230282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFEB23470</t>
   </si>
   <si>
     <t xml:space="preserve">DE4070408675</t>
   </si>
   <si>
-    <t xml:space="preserve">DEFEB23470</t>
+    <t xml:space="preserve">DE4170123108</t>
   </si>
   <si>
     <t xml:space="preserve">DE2250132994</t>
   </si>
   <si>
-    <t xml:space="preserve">DE4170123108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RU17230282</t>
-  </si>
-  <si>
     <t xml:space="preserve">FR552081317</t>
   </si>
   <si>
@@ -404,28 +413,31 @@
     <t xml:space="preserve">DE8290178515</t>
   </si>
   <si>
+    <t xml:space="preserve">GB03039100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBOC303117</t>
+  </si>
+  <si>
     <t xml:space="preserve">FR379677636</t>
   </si>
   <si>
-    <t xml:space="preserve">GBOC303117</t>
+    <t xml:space="preserve">FR*J00S1080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7330530056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IE008610</t>
   </si>
   <si>
     <t xml:space="preserve">DEFEI1007130</t>
   </si>
   <si>
-    <t xml:space="preserve">FR*J00S1080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB03039100</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE5110216866</t>
   </si>
   <si>
-    <t xml:space="preserve">DE7330530056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE008610</t>
+    <t xml:space="preserve">FR542008677</t>
   </si>
   <si>
     <t xml:space="preserve">DE8170600335</t>
@@ -437,12 +449,12 @@
     <t xml:space="preserve">DE5110001494</t>
   </si>
   <si>
-    <t xml:space="preserve">FR542008677</t>
-  </si>
-  <si>
     <t xml:space="preserve">CH0000049173</t>
   </si>
   <si>
+    <t xml:space="preserve">HU10625790</t>
+  </si>
+  <si>
     <t xml:space="preserve">DE7010228841</t>
   </si>
   <si>
@@ -452,22 +464,25 @@
     <t xml:space="preserve">DE2010198197</t>
   </si>
   <si>
-    <t xml:space="preserve">HU10625790</t>
-  </si>
-  <si>
     <t xml:space="preserve">CZ41692918</t>
   </si>
   <si>
+    <t xml:space="preserve">DEFEB13109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO912230252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2030006515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR380415125</t>
+  </si>
+  <si>
     <t xml:space="preserve">DE2010378297</t>
   </si>
   <si>
-    <t xml:space="preserve">DE2030006515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB13109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO912230252</t>
+    <t xml:space="preserve">ESG08171118</t>
   </si>
   <si>
     <t xml:space="preserve">DEFEB13306</t>
@@ -476,46 +491,43 @@
     <t xml:space="preserve">FI06353667</t>
   </si>
   <si>
-    <t xml:space="preserve">ESG08171118</t>
-  </si>
-  <si>
     <t xml:space="preserve">US341843785</t>
   </si>
   <si>
-    <t xml:space="preserve">FR380415125</t>
-  </si>
-  <si>
     <t xml:space="preserve">GB03586615</t>
   </si>
   <si>
     <t xml:space="preserve">DE*J00S1100</t>
   </si>
   <si>
+    <t xml:space="preserve">GB02366963</t>
+  </si>
+  <si>
     <t xml:space="preserve">DEFEB13172</t>
   </si>
   <si>
+    <t xml:space="preserve">DE7330029432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB02020410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB01833679</t>
+  </si>
+  <si>
     <t xml:space="preserve">DEFEB48901</t>
   </si>
   <si>
-    <t xml:space="preserve">GB02020410</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7330029432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB02366963</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE6070002888</t>
   </si>
   <si>
     <t xml:space="preserve">DEFEI1007380</t>
   </si>
   <si>
+    <t xml:space="preserve">GB03690065</t>
+  </si>
+  <si>
     <t xml:space="preserve">FI02459755</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB03690065</t>
   </si>
 </sst>
 </file>
@@ -1687,6 +1699,26 @@
         <v>167</v>
       </c>
     </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>171</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Large code update to check functionality. Excluding large data files for now. Complete and commented version will be uploaded when the written thesis is finished.
</commit_message>
<xml_diff>
--- a/BvIDexport.xlsx
+++ b/BvIDexport.xlsx
@@ -12,11 +12,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t xml:space="preserve">NewBvDIDs</t>
   </si>
   <si>
+    <t xml:space="preserve">DE7110345674</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI16700343</t>
+  </si>
+  <si>
     <t xml:space="preserve">FR542051180</t>
   </si>
   <si>
@@ -26,9 +32,6 @@
     <t xml:space="preserve">DE5330000056</t>
   </si>
   <si>
-    <t xml:space="preserve">US142546192L</t>
-  </si>
-  <si>
     <t xml:space="preserve">GB12133117</t>
   </si>
   <si>
@@ -38,7 +41,7 @@
     <t xml:space="preserve">DE5110426441</t>
   </si>
   <si>
-    <t xml:space="preserve">DE5190434206</t>
+    <t xml:space="preserve">DE6070009834</t>
   </si>
   <si>
     <t xml:space="preserve">DE4010000539</t>
@@ -47,9 +50,6 @@
     <t xml:space="preserve">DE5030088293</t>
   </si>
   <si>
-    <t xml:space="preserve">FR180020026</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE8330415355</t>
   </si>
   <si>
@@ -59,21 +59,24 @@
     <t xml:space="preserve">ESB98338411</t>
   </si>
   <si>
+    <t xml:space="preserve">CN40115PC</t>
+  </si>
+  <si>
     <t xml:space="preserve">DE2151574829</t>
   </si>
   <si>
     <t xml:space="preserve">DE5050471540</t>
   </si>
   <si>
-    <t xml:space="preserve">DE6070009834</t>
-  </si>
-  <si>
     <t xml:space="preserve">GB*908439227</t>
   </si>
   <si>
     <t xml:space="preserve">DE5050567293</t>
   </si>
   <si>
+    <t xml:space="preserve">HU10625790</t>
+  </si>
+  <si>
     <t xml:space="preserve">NO988470937</t>
   </si>
   <si>
@@ -83,12 +86,12 @@
     <t xml:space="preserve">DE5030319504</t>
   </si>
   <si>
-    <t xml:space="preserve">SE5564620887</t>
-  </si>
-  <si>
     <t xml:space="preserve">BM45532R</t>
   </si>
   <si>
+    <t xml:space="preserve">GBOC333488</t>
+  </si>
+  <si>
     <t xml:space="preserve">NO863769132</t>
   </si>
   <si>
@@ -110,12 +113,6 @@
     <t xml:space="preserve">DEFEB41239</t>
   </si>
   <si>
-    <t xml:space="preserve">DE5030456699</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFEB13116</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE2290291348</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t xml:space="preserve">DE5110426307</t>
   </si>
   <si>
-    <t xml:space="preserve">DE2370010537</t>
-  </si>
-  <si>
     <t xml:space="preserve">SE5560362138</t>
   </si>
   <si>
@@ -149,9 +143,6 @@
     <t xml:space="preserve">ESB82056748</t>
   </si>
   <si>
-    <t xml:space="preserve">SE5567818314</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE6070491599</t>
   </si>
   <si>
@@ -173,6 +164,9 @@
     <t xml:space="preserve">DE7170000175</t>
   </si>
   <si>
+    <t xml:space="preserve">DE7290514922</t>
+  </si>
+  <si>
     <t xml:space="preserve">US133413761L</t>
   </si>
   <si>
@@ -182,9 +176,6 @@
     <t xml:space="preserve">DE2011364466</t>
   </si>
   <si>
-    <t xml:space="preserve">IT04732570967</t>
-  </si>
-  <si>
     <t xml:space="preserve">CHCHE112112310</t>
   </si>
   <si>
@@ -260,6 +251,9 @@
     <t xml:space="preserve">KY31377PC</t>
   </si>
   <si>
+    <t xml:space="preserve">DE5110013057</t>
+  </si>
+  <si>
     <t xml:space="preserve">US411724239</t>
   </si>
   <si>
@@ -293,27 +287,18 @@
     <t xml:space="preserve">GBLP011863</t>
   </si>
   <si>
-    <t xml:space="preserve">IT10236451000</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE2250192021</t>
   </si>
   <si>
     <t xml:space="preserve">GB04043908</t>
   </si>
   <si>
-    <t xml:space="preserve">DE2350113248</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE8310297852</t>
   </si>
   <si>
     <t xml:space="preserve">CHCHE114669799</t>
   </si>
   <si>
-    <t xml:space="preserve">AT9150100345</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE2011425555</t>
   </si>
   <si>
@@ -323,96 +308,81 @@
     <t xml:space="preserve">LULB104637</t>
   </si>
   <si>
+    <t xml:space="preserve">DE7110175411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBGG50009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2230133950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE7330620677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE*929123061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL34108286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE0403170701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE2190331916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ00260428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE6290207493</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS6306051210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU00040778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO987059699</t>
+  </si>
+  <si>
     <t xml:space="preserve">IT00811720580</t>
   </si>
   <si>
-    <t xml:space="preserve">DE7110175411</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBGG50009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2230133950</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KY*110179911376</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7330620677</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NL01178978</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE*929123061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NL34108286</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE2190331916</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ00260428</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE6290207493</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IS6306051210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RU00040778</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO987059699</t>
-  </si>
-  <si>
     <t xml:space="preserve">GB02989338</t>
   </si>
   <si>
-    <t xml:space="preserve">DE2250063387</t>
+    <t xml:space="preserve">DE6070524807</t>
   </si>
   <si>
     <t xml:space="preserve">DE7370113108</t>
   </si>
   <si>
-    <t xml:space="preserve">DE2050488817</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE6070524807</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US363145972</t>
-  </si>
-  <si>
     <t xml:space="preserve">RU17230282</t>
   </si>
   <si>
+    <t xml:space="preserve">DE4070408675</t>
+  </si>
+  <si>
     <t xml:space="preserve">DEFEB23470</t>
   </si>
   <si>
-    <t xml:space="preserve">DE4070408675</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE4170123108</t>
   </si>
   <si>
-    <t xml:space="preserve">DE2250132994</t>
-  </si>
-  <si>
     <t xml:space="preserve">FR552081317</t>
   </si>
   <si>
-    <t xml:space="preserve">DEFEB13584</t>
-  </si>
-  <si>
     <t xml:space="preserve">US149185809L</t>
   </si>
   <si>
     <t xml:space="preserve">DE8290178515</t>
   </si>
   <si>
+    <t xml:space="preserve">FR*J00S1080</t>
+  </si>
+  <si>
     <t xml:space="preserve">GB03039100</t>
   </si>
   <si>
@@ -422,9 +392,6 @@
     <t xml:space="preserve">FR379677636</t>
   </si>
   <si>
-    <t xml:space="preserve">FR*J00S1080</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE7330530056</t>
   </si>
   <si>
@@ -449,10 +416,7 @@
     <t xml:space="preserve">DE5110001494</t>
   </si>
   <si>
-    <t xml:space="preserve">CH0000049173</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HU10625790</t>
+    <t xml:space="preserve">DE2150055529</t>
   </si>
   <si>
     <t xml:space="preserve">DE7010228841</t>
@@ -482,9 +446,6 @@
     <t xml:space="preserve">DE2010378297</t>
   </si>
   <si>
-    <t xml:space="preserve">ESG08171118</t>
-  </si>
-  <si>
     <t xml:space="preserve">DEFEB13306</t>
   </si>
   <si>
@@ -500,13 +461,7 @@
     <t xml:space="preserve">DE*J00S1100</t>
   </si>
   <si>
-    <t xml:space="preserve">GB02366963</t>
-  </si>
-  <si>
     <t xml:space="preserve">DEFEB13172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE7330029432</t>
   </si>
   <si>
     <t xml:space="preserve">GB02020410</t>
@@ -1644,81 +1599,6 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158">
-      <c r="A158" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="s">
-        <v>171</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>